<commit_message>
test updates because of change to tax calc
</commit_message>
<xml_diff>
--- a/tests/DISCK.xlsx
+++ b/tests/DISCK.xlsx
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="B3" s="28" t="n">
-        <v>45265</v>
+        <v>45621</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="18">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="B11" s="30" t="n">
-        <v>146.8875219993258</v>
+        <v>146.8567227010758</v>
       </c>
     </row>
     <row r="12" ht="13.8" customHeight="1" s="18">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="B17" s="31" t="n">
-        <v>128.7489388630488</v>
+        <v>128.6959462351709</v>
       </c>
     </row>
     <row r="18" ht="13.8" customHeight="1" s="18">
@@ -7276,13 +7276,13 @@
         <v>0.722295</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8138597249999999</v>
+        <v>0.81345984825</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9292499999999997</v>
+        <v>0.9292499999999998</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9683624999999999</v>
+        <v>0.9683625</v>
       </c>
       <c r="G7" t="n">
         <v>1.612987060746391</v>
@@ -7353,7 +7353,7 @@
         <v>51.7</v>
       </c>
       <c r="C9" t="n">
-        <v>43.45350000000001</v>
+        <v>43.482795</v>
       </c>
       <c r="D9" t="n">
         <v>35</v>
@@ -7396,7 +7396,7 @@
         <v>3.3605</v>
       </c>
       <c r="D10" t="n">
-        <v>2.8244775</v>
+        <v>2.826381675</v>
       </c>
       <c r="E10" t="n">
         <v>2.275</v>
@@ -7433,34 +7433,34 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>3.108624468950438e-15</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3081627749999973</v>
+        <v>0.2773634767499966</v>
       </c>
       <c r="E11" t="n">
-        <v>11.953912775</v>
+        <v>11.92311347675</v>
       </c>
       <c r="F11" t="n">
-        <v>26.046800275</v>
+        <v>26.01600097674999</v>
       </c>
       <c r="G11" t="n">
-        <v>43.1838132142536</v>
+        <v>43.1530139160036</v>
       </c>
       <c r="H11" t="n">
-        <v>59.48825159276083</v>
+        <v>59.45745229451082</v>
       </c>
       <c r="I11" t="n">
-        <v>77.42414041052166</v>
+        <v>77.39334111227166</v>
       </c>
       <c r="J11" t="n">
-        <v>97.8479671675361</v>
+        <v>97.8171678692861</v>
       </c>
       <c r="K11" t="n">
-        <v>120.6615443638041</v>
+        <v>120.6307450655541</v>
       </c>
       <c r="L11" t="n">
-        <v>146.8875219993258</v>
+        <v>146.8567227010758</v>
       </c>
     </row>
     <row r="12">
@@ -7556,31 +7556,31 @@
         <v>2.3</v>
       </c>
       <c r="D14" t="n">
-        <v>2.290529780118272</v>
+        <v>2.291472942632959</v>
       </c>
       <c r="E14" t="n">
-        <v>1.991519398107974</v>
+        <v>1.992339438283776</v>
       </c>
       <c r="F14" t="n">
-        <v>1.706424618927786</v>
+        <v>1.707127266738211</v>
       </c>
       <c r="G14" t="n">
-        <v>1.447498777173317</v>
+        <v>1.448094808099672</v>
       </c>
       <c r="H14" t="n">
-        <v>1.251421942753264</v>
+        <v>1.251937235886192</v>
       </c>
       <c r="I14" t="n">
-        <v>1.081154014481897</v>
+        <v>1.081599197054031</v>
       </c>
       <c r="J14" t="n">
-        <v>0.9306935103584705</v>
+        <v>0.9310767383956051</v>
       </c>
       <c r="K14" t="n">
-        <v>0.8010869668899998</v>
+        <v>0.8014168273461849</v>
       </c>
       <c r="L14" t="n">
-        <v>0.8010869668899998</v>
+        <v>0.8014168273461849</v>
       </c>
     </row>
     <row r="15">
@@ -7593,34 +7593,34 @@
         <v>28.22</v>
       </c>
       <c r="C15" t="n">
-        <v>32.54019218651544</v>
+        <v>32.5274552299937</v>
       </c>
       <c r="D15" t="n">
-        <v>38.94764429817995</v>
+        <v>38.93161357948631</v>
       </c>
       <c r="E15" t="n">
-        <v>49.43228894098033</v>
+        <v>49.41194277800501</v>
       </c>
       <c r="F15" t="n">
-        <v>66.1850235694284</v>
+        <v>66.15778203752855</v>
       </c>
       <c r="G15" t="n">
-        <v>83.15331296902906</v>
+        <v>83.11908734658975</v>
       </c>
       <c r="H15" t="n">
-        <v>105.3392086216921</v>
+        <v>105.2958513596226</v>
       </c>
       <c r="I15" t="n">
-        <v>135.7421130282821</v>
+        <v>135.6862420335648</v>
       </c>
       <c r="J15" t="n">
-        <v>176.0218009503347</v>
+        <v>175.9493509722724</v>
       </c>
       <c r="K15" t="n">
-        <v>230.881788056533</v>
+        <v>230.7867578932841</v>
       </c>
       <c r="L15" t="n">
-        <v>230.881788056533</v>
+        <v>230.7867578932841</v>
       </c>
     </row>
     <row r="16">
@@ -7673,10 +7673,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>3.108624468950438e-15</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3081627749999942</v>
+        <v>0.2773634767499971</v>
       </c>
       <c r="E17" t="n">
         <v>11.64575</v>
@@ -7753,10 +7753,10 @@
         <v>8.02</v>
       </c>
       <c r="C19" t="n">
-        <v>3.108624468950438e-15</v>
+        <v>-4.440892098500626e-16</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3081627749999942</v>
+        <v>0.2773634767499971</v>
       </c>
       <c r="E19" t="n">
         <v>11.64575</v>
@@ -7793,7 +7793,7 @@
         <v>10.864</v>
       </c>
       <c r="C20" t="n">
-        <v>10.901295</v>
+        <v>10.872</v>
       </c>
       <c r="D20" t="n">
         <v>10.993</v>
@@ -7833,10 +7833,10 @@
         <v>8.02</v>
       </c>
       <c r="C21" t="n">
-        <v>8.246500000000001</v>
+        <v>8.217205</v>
       </c>
       <c r="D21" t="n">
-        <v>8.761662775</v>
+        <v>8.76015847675</v>
       </c>
       <c r="E21" t="n">
         <v>9.89575</v>
@@ -7900,7 +7900,7 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>32.7379906545438</v>
+        <v>32.72451580829226</v>
       </c>
     </row>
     <row r="23">
@@ -7916,7 +7916,7 @@
         <v>3.4395</v>
       </c>
       <c r="D23" t="n">
-        <v>3.8755225</v>
+        <v>3.873618325</v>
       </c>
       <c r="E23" t="n">
         <v>4.424999999999999</v>
@@ -7953,10 +7953,10 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>-8.246499999999997</v>
+        <v>-8.217205</v>
       </c>
       <c r="D24" t="n">
-        <v>-8.453500000000005</v>
+        <v>-8.482795000000003</v>
       </c>
       <c r="E24" t="n">
         <v>1.75</v>
@@ -7993,16 +7993,16 @@
         <v>0.68</v>
       </c>
       <c r="C25" t="n">
-        <v>0.6929999999999998</v>
+        <v>0.722295</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8138597249999999</v>
+        <v>0.81345984825</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9292499999999997</v>
+        <v>0.9292499999999998</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9683624999999999</v>
+        <v>0.9683625</v>
       </c>
       <c r="G25" t="n">
         <v>1.612987060746391</v>
@@ -8036,7 +8036,7 @@
         <v>3.4395</v>
       </c>
       <c r="D26" t="n">
-        <v>3.8755225</v>
+        <v>3.873618325</v>
       </c>
       <c r="E26" t="n">
         <v>4.424999999999999</v>
@@ -8150,10 +8150,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>170.0201968141328</v>
+        <v>169.994742848637</v>
       </c>
       <c r="C29" t="n">
-        <v>187.0222164955461</v>
+        <v>186.9942171335007</v>
       </c>
       <c r="D29" t="n">
         <v>205.4162753701008</v>
@@ -8190,10 +8190,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>221.7201968141329</v>
+        <v>221.694742848637</v>
       </c>
       <c r="C30" t="n">
-        <v>230.4757164955461</v>
+        <v>230.4770121335007</v>
       </c>
       <c r="D30" t="n">
         <v>240.4162753701008</v>
@@ -8230,10 +8230,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.08865594999399858</v>
+        <v>0.08865464752261958</v>
       </c>
       <c r="C31" t="n">
-        <v>0.09082761165842454</v>
+        <v>0.09082147951690445</v>
       </c>
       <c r="D31" t="n">
         <v>0.09291749280543192</v>
@@ -8270,10 +8270,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>222.7035911071141</v>
+        <v>222.6781438463931</v>
       </c>
       <c r="C32" t="n">
-        <v>231.5462945437903</v>
+        <v>231.5475962000862</v>
       </c>
       <c r="D32" t="n">
         <v>241.5840914655608</v>
@@ -8310,37 +8310,37 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>128.7489388630488</v>
+        <v>128.6959462351709</v>
       </c>
       <c r="C33" t="n">
-        <v>141.6238327493537</v>
+        <v>141.5655408586879</v>
       </c>
       <c r="D33" t="n">
-        <v>155.7862160242891</v>
+        <v>155.7220949445567</v>
       </c>
       <c r="E33" t="n">
-        <v>171.364837626718</v>
+        <v>171.2943044390124</v>
       </c>
       <c r="F33" t="n">
-        <v>188.5013213893899</v>
+        <v>188.4237348829137</v>
       </c>
       <c r="G33" t="n">
-        <v>207.3514535283288</v>
+        <v>207.266108371205</v>
       </c>
       <c r="H33" t="n">
-        <v>228.0865988811618</v>
+        <v>227.9927192083256</v>
       </c>
       <c r="I33" t="n">
-        <v>250.8952587692779</v>
+        <v>250.7919911291581</v>
       </c>
       <c r="J33" t="n">
-        <v>275.9847846462058</v>
+        <v>275.871190242074</v>
       </c>
       <c r="K33" t="n">
-        <v>303.5832631108264</v>
+        <v>303.4583092662814</v>
       </c>
       <c r="L33" t="n">
-        <v>301.2035987673652</v>
+        <v>301.0796243846173</v>
       </c>
     </row>
     <row r="34">
@@ -8350,10 +8350,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>73.92182470179689</v>
+        <v>73.91075776027695</v>
       </c>
       <c r="C34" t="n">
-        <v>81.31400717197658</v>
+        <v>81.30183353630466</v>
       </c>
       <c r="D34" t="n">
         <v>89.31142407395687</v>
@@ -8390,37 +8390,37 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>128.7489388630488</v>
+        <v>128.6959462351709</v>
       </c>
       <c r="C35" t="n">
-        <v>141.6238327493537</v>
+        <v>141.5655408586879</v>
       </c>
       <c r="D35" t="n">
-        <v>155.7862160242891</v>
+        <v>155.7220949445567</v>
       </c>
       <c r="E35" t="n">
-        <v>171.364837626718</v>
+        <v>171.2943044390124</v>
       </c>
       <c r="F35" t="n">
-        <v>188.5013213893899</v>
+        <v>188.4237348829137</v>
       </c>
       <c r="G35" t="n">
-        <v>207.3514535283288</v>
+        <v>207.266108371205</v>
       </c>
       <c r="H35" t="n">
-        <v>228.0865988811618</v>
+        <v>227.9927192083256</v>
       </c>
       <c r="I35" t="n">
-        <v>250.8952587692779</v>
+        <v>250.7919911291581</v>
       </c>
       <c r="J35" t="n">
-        <v>275.9847846462058</v>
+        <v>275.871190242074</v>
       </c>
       <c r="K35" t="n">
-        <v>303.5832631108264</v>
+        <v>303.4583092662814</v>
       </c>
       <c r="L35" t="n">
-        <v>301.2035987673652</v>
+        <v>301.0796243846173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>